<commit_message>
Add invoicing periods bounds to example 03
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/03-fixed-hours-per-task/03-fixed-hours-per-task.xlsx
+++ b/ampl-data-input-excel/03-fixed-hours-per-task/03-fixed-hours-per-task.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="89">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -707,7 +707,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D3:D6 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -782,8 +782,8 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -808,29 +808,74 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
@@ -866,7 +911,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D3:D6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -903,7 +948,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="1" sqref="D3:D6 F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -961,7 +1006,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="D3:D6 F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1060,7 +1105,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="D3:D6 F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1158,7 +1203,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="D3:D6 F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1243,8 +1288,8 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="D3:D6 H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1315,7 +1360,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D3:D6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1386,7 +1431,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D3:D6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1477,7 +1522,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D3:D6 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1729,7 +1774,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="D3:D6 B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1885,7 +1930,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="D3:D6 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2558,7 +2603,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="D3:D6 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2953,7 +2998,7 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D3:D6 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3417,7 +3462,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="D3:D6 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3812,7 +3857,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D3:D6 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4009,7 +4054,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D3:D6 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add invoicing periods bounds to example 03, 04
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/03-fixed-hours-per-task/03-fixed-hours-per-task.xlsx
+++ b/ampl-data-input-excel/03-fixed-hours-per-task/03-fixed-hours-per-task.xlsx
@@ -707,7 +707,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D3:D6 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -783,7 +783,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3:D6"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -911,7 +911,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D3:D6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -948,7 +948,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="1" sqref="D3:D6 F21"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1006,7 +1006,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="D3:D6 F3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1105,7 +1105,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="D3:D6 F3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1203,7 +1203,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="D3:D6 F3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1289,7 +1289,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="D3:D6 H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1360,7 +1360,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D3:D6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1431,7 +1431,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D3:D6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1522,7 +1522,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D3:D6 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1774,7 +1774,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="D3:D6 B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1930,7 +1930,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="D3:D6 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2603,7 +2603,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="D3:D6 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2998,7 +2998,7 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D3:D6 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3462,7 +3462,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="D3:D6 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3857,7 +3857,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D3:D6 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4054,7 +4054,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D3:D6 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>